<commit_message>
TESTS: tweaking tests for new RNGs
</commit_message>
<xml_diff>
--- a/psychopy/tests/data/corrXlsx.xlsx
+++ b/psychopy/tests/data/corrXlsx.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpzjwp/code/psychopy/git/psychopy/tests/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0D03FB-693D-3947-A13E-D9299002B56C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-9840" yWindow="-18800" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="rawData" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="rawData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>text</t>
   </si>
@@ -65,20 +70,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,15 +98,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -390,20 +403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +434,6 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s"/>
       <c r="I1" t="s">
         <v>7</v>
       </c>
@@ -435,294 +443,290 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s"/>
       <c r="M1" t="s">
         <v>10</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O2" t="n">
-        <v>9</v>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="J2">
+        <v>0.20000000298023221</v>
+      </c>
+      <c r="K2">
+        <v>0.30000001192092901</v>
+      </c>
+      <c r="L2">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="M2">
+        <v>0.14142136361300811</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s"/>
-      <c r="H3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="K3" t="s"/>
-      <c r="L3" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="K3">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="L3">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.414213562373095</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.300000011920929</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.1414213636130081</v>
-      </c>
-      <c r="N4" t="n">
-        <v>3</v>
-      </c>
-      <c r="O4" t="n">
-        <v>6</v>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="J4">
+        <v>0.15000000596046451</v>
+      </c>
+      <c r="K4">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="L4">
+        <v>0.20000000298023221</v>
+      </c>
+      <c r="M4">
+        <v>7.0710679172326166E-2</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.7071067811865476</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.300000011920929</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.07071068444068282</v>
-      </c>
-      <c r="N5" t="n">
-        <v>5</v>
-      </c>
-      <c r="O5" t="n">
-        <v>8</v>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="J5">
+        <v>0.15000000596046451</v>
+      </c>
+      <c r="K5">
+        <v>0.20000000298023221</v>
+      </c>
+      <c r="L5">
+        <v>0.10000000149011611</v>
+      </c>
+      <c r="M5">
+        <v>7.0710679172326166E-2</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>11</v>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.30000001192092901</v>
+      </c>
+      <c r="L6">
+        <v>0.30000001192092901</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2.5</v>
+      </c>
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="I7" t="n">
-        <v>1.414213562373095</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.2000000029802322</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.1000000014901161</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.300000011920929</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.1414213636130081</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
-        <v>7</v>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="J7">
+        <v>0.25</v>
+      </c>
+      <c r="K7">
+        <v>0.30000001192092901</v>
+      </c>
+      <c r="L7">
+        <v>0.20000000298023221</v>
+      </c>
+      <c r="M7">
+        <v>7.0710684440682819E-2</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>